<commit_message>
XLS and XLSX conversions now use agate-excel. Closes #493.
</commit_message>
<xml_diff>
--- a/examples/sheets.xlsx
+++ b/examples/sheets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="22840" windowHeight="12660" tabRatio="427" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="274" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="testfixed_converted.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="not this one" sheetId="2" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>text</t>
   </si>
@@ -37,9 +37,6 @@
     <t>float</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
@@ -62,19 +59,15 @@
   </si>
   <si>
     <t>Unicode! Σ</t>
-  </si>
-  <si>
-    <t>Extra data past headers will be trimmed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -104,12 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -560,21 +552,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" customWidth="1"/>
+    <col min="6" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,13 +606,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>24472</v>
@@ -618,15 +625,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="4">
-        <v>0.1763888888888889</v>
-      </c>
-      <c r="G2" s="5">
         <v>24472.176388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>16071</v>
@@ -642,18 +646,15 @@
         <v>1.27</v>
       </c>
       <c r="F3" s="4">
-        <v>0.62306712962962962</v>
-      </c>
-      <c r="G3" s="5">
         <v>16071.623067129629</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>5844</v>
@@ -669,20 +670,17 @@
         <v>41800000.009999998</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
         <v>5844</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -695,142 +693,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5844</v>
-      </c>
-      <c r="C2">
-        <v>164</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>41800000.009999998</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>5844</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>16071</v>
-      </c>
-      <c r="C3">
-        <v>63</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1.27</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.62306712962962962</v>
-      </c>
-      <c r="G3" s="5">
-        <v>16071.623067129629</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1">
-        <v>24472</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.1763888888888889</v>
-      </c>
-      <c r="G4" s="5">
-        <v>24472.176388888889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
in2csv accepts utf-8 arguments to the --sheet option in Python 2
</commit_message>
<xml_diff>
--- a/examples/sheets.xlsx
+++ b/examples/sheets.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Sites/shared/pulls/csvkit/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="274" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="274" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="not this one" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
+    <sheet name="ʤ" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -20,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>text</t>
   </si>
@@ -59,6 +68,15 @@
   </si>
   <si>
     <t>Unicode! Σ</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -68,7 +86,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -102,7 +120,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,6 +195,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -486,7 +509,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -530,7 +553,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -556,14 +579,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -571,20 +589,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="6" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" customWidth="1"/>
+    <col min="6" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -628,7 +644,7 @@
         <v>24472.176388888889</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -652,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -673,12 +689,12 @@
         <v>5844</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -687,10 +703,40 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>